<commit_message>
add mudanças na função do match de dados
</commit_message>
<xml_diff>
--- a/SMTR202211008775_844_2022-11-30/data/output/analise_amostra_pre_solucao.xlsx
+++ b/SMTR202211008775_844_2022-11-30/data/output/analise_amostra_pre_solucao.xlsx
@@ -445,7 +445,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>servico</t>
+          <t>servico_amostra</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -485,27 +485,27 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>servico_informado</t>
+          <t>id_veiculo_apurado</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>id_veiculo_apurada</t>
+          <t>servico_apurado</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>sentido_apurada</t>
+          <t>sentido_apurado</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>datetime_partida_apurada</t>
+          <t>datetime_partida_apurado</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>datetime_chegada_apurada</t>
+          <t>datetime_chegada_apurado</t>
         </is>
       </c>
     </row>
@@ -1269,17 +1269,17 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -4709,17 +4709,17 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
@@ -5539,17 +5539,17 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L112" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M112" t="inlineStr">
@@ -6729,17 +6729,17 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M138" t="inlineStr">
@@ -6794,17 +6794,17 @@
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M139" t="inlineStr">
@@ -6859,17 +6859,17 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
@@ -6924,17 +6924,17 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M141" t="inlineStr">
@@ -6989,17 +6989,17 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M142" t="inlineStr">
@@ -7054,17 +7054,17 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
@@ -7119,17 +7119,17 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M144" t="inlineStr">
@@ -7184,17 +7184,17 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
@@ -7249,17 +7249,17 @@
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
@@ -7314,17 +7314,17 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -7379,17 +7379,17 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
@@ -7444,17 +7444,17 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
@@ -7509,17 +7509,17 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
@@ -7574,17 +7574,17 @@
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M151" t="inlineStr">
@@ -7639,17 +7639,17 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M152" t="inlineStr">
@@ -7704,17 +7704,17 @@
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M153" t="inlineStr">
@@ -7769,17 +7769,17 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M154" t="inlineStr">
@@ -7834,17 +7834,17 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M155" t="inlineStr">
@@ -7899,17 +7899,17 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M156" t="inlineStr">
@@ -7964,17 +7964,17 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -8029,17 +8029,17 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M158" t="inlineStr">
@@ -8094,17 +8094,17 @@
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M159" t="inlineStr">
@@ -8159,17 +8159,17 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M160" t="inlineStr">
@@ -8224,17 +8224,17 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M161" t="inlineStr">
@@ -8289,17 +8289,17 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M162" t="inlineStr">
@@ -8354,17 +8354,17 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
@@ -8419,17 +8419,17 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M164" t="inlineStr">
@@ -8484,17 +8484,17 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M165" t="inlineStr">
@@ -8549,17 +8549,17 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M166" t="inlineStr">
@@ -8614,17 +8614,17 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M167" t="inlineStr">
@@ -8679,17 +8679,17 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M168" t="inlineStr">
@@ -8744,17 +8744,17 @@
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M169" t="inlineStr">
@@ -8809,17 +8809,17 @@
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M170" t="inlineStr">
@@ -8874,17 +8874,17 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M171" t="inlineStr">
@@ -8939,17 +8939,17 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M172" t="inlineStr">
@@ -9004,17 +9004,17 @@
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M173" t="inlineStr">
@@ -9069,17 +9069,17 @@
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M174" t="inlineStr">
@@ -9134,17 +9134,17 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M175" t="inlineStr">
@@ -9199,17 +9199,17 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M176" t="inlineStr">
@@ -9264,17 +9264,17 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M177" t="inlineStr">
@@ -9329,17 +9329,17 @@
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M178" t="inlineStr">
@@ -9394,17 +9394,17 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M179" t="inlineStr">
@@ -9459,17 +9459,17 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M180" t="inlineStr">
@@ -9524,17 +9524,17 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M181" t="inlineStr">
@@ -9589,17 +9589,17 @@
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K182" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M182" t="inlineStr">
@@ -9654,17 +9654,17 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M183" t="inlineStr">
@@ -9719,17 +9719,17 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M184" t="inlineStr">
@@ -9784,17 +9784,17 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M185" t="inlineStr">
@@ -9849,17 +9849,17 @@
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M186" t="inlineStr">
@@ -9914,7 +9914,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>Viagem circular inválida - sem sinal inicial/final dentro do raio de 500m (inclui o caso acima em que o veículo fez apenas metade do trajeto).</t>
+          <t>Viagem circular inválida - sem sinal inicial/final dentro do raio de 500m</t>
         </is>
       </c>
       <c r="K187" t="inlineStr"/>
@@ -9963,17 +9963,17 @@
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M188" t="inlineStr">
@@ -10028,17 +10028,17 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M189" t="inlineStr">
@@ -10093,17 +10093,17 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M190" t="inlineStr">
@@ -10158,17 +10158,17 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M191" t="inlineStr">
@@ -10223,17 +10223,17 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L192" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M192" t="inlineStr">
@@ -10288,17 +10288,17 @@
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L193" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M193" t="inlineStr">
@@ -10353,17 +10353,17 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M194" t="inlineStr">
@@ -10418,17 +10418,17 @@
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L195" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M195" t="inlineStr">
@@ -10483,17 +10483,17 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M196" t="inlineStr">
@@ -10548,17 +10548,17 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M197" t="inlineStr">
@@ -10613,17 +10613,17 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L198" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M198" t="inlineStr">
@@ -10678,17 +10678,17 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L199" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M199" t="inlineStr">
@@ -10743,17 +10743,17 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L200" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M200" t="inlineStr">
@@ -10808,17 +10808,17 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L201" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M201" t="inlineStr">
@@ -10873,17 +10873,17 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M202" t="inlineStr">
@@ -10938,17 +10938,17 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M203" t="inlineStr">
@@ -11003,17 +11003,17 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M204" t="inlineStr">
@@ -11068,17 +11068,17 @@
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L205" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M205" t="inlineStr">
@@ -11133,17 +11133,17 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M206" t="inlineStr">
@@ -11198,17 +11198,17 @@
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M207" t="inlineStr">
@@ -11263,17 +11263,17 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L208" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M208" t="inlineStr">
@@ -11328,17 +11328,17 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M209" t="inlineStr">
@@ -11393,17 +11393,17 @@
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K210" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L210" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M210" t="inlineStr">
@@ -11458,17 +11458,17 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L211" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M211" t="inlineStr">
@@ -11523,17 +11523,17 @@
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K212" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M212" t="inlineStr">
@@ -11588,17 +11588,17 @@
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K213" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M213" t="inlineStr">
@@ -11653,17 +11653,17 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L214" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M214" t="inlineStr">
@@ -11718,17 +11718,17 @@
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K215" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M215" t="inlineStr">
@@ -11783,17 +11783,17 @@
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L216" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M216" t="inlineStr">
@@ -11848,17 +11848,17 @@
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K217" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L217" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M217" t="inlineStr">
@@ -11913,17 +11913,17 @@
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L218" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M218" t="inlineStr">
@@ -11978,17 +11978,17 @@
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L219" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M219" t="inlineStr">
@@ -12043,17 +12043,17 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K220" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L220" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M220" t="inlineStr">
@@ -12108,17 +12108,17 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M221" t="inlineStr">
@@ -12173,17 +12173,17 @@
       </c>
       <c r="J222" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K222" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M222" t="inlineStr">
@@ -12238,17 +12238,17 @@
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L223" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M223" t="inlineStr">
@@ -12303,17 +12303,17 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M224" t="inlineStr">
@@ -12368,17 +12368,17 @@
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L225" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M225" t="inlineStr">
@@ -12433,17 +12433,17 @@
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M226" t="inlineStr">
@@ -12498,17 +12498,17 @@
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M227" t="inlineStr">
@@ -12563,17 +12563,17 @@
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L228" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M228" t="inlineStr">
@@ -12628,17 +12628,17 @@
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M229" t="inlineStr">
@@ -12693,17 +12693,17 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M230" t="inlineStr">
@@ -12758,17 +12758,17 @@
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K231" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L231" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M231" t="inlineStr">
@@ -12823,17 +12823,17 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M232" t="inlineStr">
@@ -12888,17 +12888,17 @@
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K233" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L233" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M233" t="inlineStr">
@@ -12953,17 +12953,17 @@
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M234" t="inlineStr">
@@ -13018,17 +13018,17 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M235" t="inlineStr">
@@ -13083,17 +13083,17 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K236" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L236" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M236" t="inlineStr">
@@ -13197,17 +13197,17 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K238" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L238" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M238" t="inlineStr">
@@ -13262,17 +13262,17 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M239" t="inlineStr">
@@ -13327,17 +13327,17 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L240" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M240" t="inlineStr">
@@ -13392,17 +13392,17 @@
       </c>
       <c r="J241" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K241" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L241" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M241" t="inlineStr">
@@ -13457,17 +13457,17 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M242" t="inlineStr">
@@ -13522,17 +13522,17 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M243" t="inlineStr">
@@ -13587,17 +13587,17 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L244" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M244" t="inlineStr">
@@ -13652,17 +13652,17 @@
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K245" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L245" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M245" t="inlineStr">
@@ -13717,17 +13717,17 @@
       </c>
       <c r="J246" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L246" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M246" t="inlineStr">
@@ -13782,17 +13782,17 @@
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K247" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L247" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M247" t="inlineStr">
@@ -13847,17 +13847,17 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K248" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M248" t="inlineStr">
@@ -13912,17 +13912,17 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M249" t="inlineStr">
@@ -13977,17 +13977,17 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M250" t="inlineStr">
@@ -14042,17 +14042,17 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K251" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M251" t="inlineStr">
@@ -14107,17 +14107,17 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K252" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M252" t="inlineStr">
@@ -14172,17 +14172,17 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M253" t="inlineStr">
@@ -14237,17 +14237,17 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K254" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M254" t="inlineStr">
@@ -14302,17 +14302,17 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L255" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M255" t="inlineStr">
@@ -14367,17 +14367,17 @@
       </c>
       <c r="J256" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K256" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M256" t="inlineStr">
@@ -14432,17 +14432,17 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K257" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L257" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M257" t="inlineStr">
@@ -14497,17 +14497,17 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M258" t="inlineStr">
@@ -14562,17 +14562,17 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M259" t="inlineStr">
@@ -14627,17 +14627,17 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M260" t="inlineStr">
@@ -14692,17 +14692,17 @@
       </c>
       <c r="J261" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K261" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L261" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M261" t="inlineStr">
@@ -14757,17 +14757,17 @@
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M262" t="inlineStr">
@@ -14822,17 +14822,17 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K263" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M263" t="inlineStr">
@@ -14887,17 +14887,17 @@
       </c>
       <c r="J264" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M264" t="inlineStr">
@@ -14952,17 +14952,17 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K265" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M265" t="inlineStr">
@@ -15017,17 +15017,17 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K266" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L266" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M266" t="inlineStr">
@@ -15082,17 +15082,17 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K267" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M267" t="inlineStr">
@@ -15147,17 +15147,17 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K268" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L268" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M268" t="inlineStr">
@@ -15212,17 +15212,17 @@
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K269" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M269" t="inlineStr">
@@ -15277,17 +15277,17 @@
       </c>
       <c r="J270" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K270" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L270" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M270" t="inlineStr">
@@ -15342,17 +15342,17 @@
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K271" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L271" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M271" t="inlineStr">
@@ -15407,17 +15407,17 @@
       </c>
       <c r="J272" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M272" t="inlineStr">
@@ -15472,17 +15472,17 @@
       </c>
       <c r="J273" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K273" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L273" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M273" t="inlineStr">
@@ -15537,17 +15537,17 @@
       </c>
       <c r="J274" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L274" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M274" t="inlineStr">
@@ -15602,17 +15602,17 @@
       </c>
       <c r="J275" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L275" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M275" t="inlineStr">
@@ -15667,17 +15667,17 @@
       </c>
       <c r="J276" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M276" t="inlineStr">
@@ -15732,17 +15732,17 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K277" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L277" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M277" t="inlineStr">
@@ -15797,17 +15797,17 @@
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K278" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L278" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M278" t="inlineStr">
@@ -15862,17 +15862,17 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>O veículo existe e operou na linha indicada pelo recurso</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L279" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M279" t="inlineStr">
@@ -15927,17 +15927,17 @@
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>novo_status</t>
+          <t>Viagem circular identificada e já paga</t>
         </is>
       </c>
       <c r="K280" t="inlineStr">
         <is>
-          <t>844</t>
+          <t>47689</t>
         </is>
       </c>
       <c r="L280" t="inlineStr">
         <is>
-          <t>47689</t>
+          <t>844</t>
         </is>
       </c>
       <c r="M280" t="inlineStr">
@@ -15992,7 +15992,7 @@
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>Viagem circular inválida - sem sinal inicial/final dentro do raio de 500m (inclui o caso acima em que o veículo fez apenas metade do trajeto).</t>
+          <t>Viagem circular inválida - sem sinal inicial/final dentro do raio de 500m</t>
         </is>
       </c>
       <c r="K281" t="inlineStr"/>

</xml_diff>